<commit_message>
Updates to figures, tables and manuscript
</commit_message>
<xml_diff>
--- a/tables/Table_3.xlsx
+++ b/tables/Table_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\Desktop\Repo\moraine-paper-2020\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70807BDF-7820-499C-BF8E-4AB6DF5773DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D378B6C5-8818-44C4-B6BC-13B4C10873AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -341,6 +341,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -424,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -465,6 +468,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -826,7 +832,7 @@
   <dimension ref="B2:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,20 +852,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
       <c r="P2" s="14"/>
@@ -870,24 +876,24 @@
     <row r="3" spans="2:20" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="19" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="19"/>
+      <c r="I3" s="20"/>
       <c r="J3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="T3" s="8"/>
@@ -952,7 +958,9 @@
       <c r="G5" s="3">
         <v>25</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="16">
+        <v>21.566510000000001</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6" t="s">
         <v>10</v>
@@ -989,7 +997,9 @@
       <c r="G6" s="3">
         <v>20</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="16">
+        <v>23.861560000000001</v>
+      </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6" t="s">
         <v>10</v>
@@ -1024,7 +1034,9 @@
       <c r="G7" s="3">
         <v>25</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="16">
+        <v>59.467800000000004</v>
+      </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6">
         <v>7</v>
@@ -1059,7 +1071,9 @@
       <c r="G8" s="3">
         <v>40</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="16">
+        <v>66.31362</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="J8" s="6" t="s">
         <v>10</v>
@@ -1094,7 +1108,9 @@
       <c r="G9" s="3">
         <v>13</v>
       </c>
-      <c r="H9" s="3"/>
+      <c r="H9" s="16">
+        <v>51.103940000000001</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6">
         <v>1</v>
@@ -1111,20 +1127,20 @@
       <c r="R9" s="3"/>
     </row>
     <row r="10" spans="2:20" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
@@ -1204,14 +1220,14 @@
       <c r="O20" s="3"/>
     </row>
     <row r="21" spans="8:15" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Updates to manuscript and figures based on co-author comments (IB, CMD, RP, AR, PH
</commit_message>
<xml_diff>
--- a/tables/Table_3.xlsx
+++ b/tables/Table_3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\Desktop\Repo\moraine-paper-2020\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC300654-534D-4B81-8A55-4E320B406962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A9C3D9-4752-4520-B854-0EEEA043FAE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Tallada</t>
   </si>
@@ -189,6 +189,44 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Table 3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>Spatial statistics for the sampled moraines</t>
+    </r>
+  </si>
+  <si>
+    <t>Number of samples</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I </t>
+  </si>
+  <si>
+    <r>
+      <t>NA</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>a</t>
     </r>
     <r>
@@ -292,36 +330,36 @@
         <rFont val="Gill Sans MT"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> 0.05 are consistent with a non-random distribution and spatial clustering of the input data.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Table 3. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>Spatial statistics for the sampled moraines</t>
-    </r>
-  </si>
-  <si>
-    <t>Number of samples</t>
-  </si>
-  <si>
-    <t>Total</t>
+      <t xml:space="preserve"> 0.05 are consistent with a non-random distribution and spatial clustering of the input data, </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Spatial autocorrelation was not possible for the Outer Pleta Naua moraine as all boulders were classed as "good" based on the 2σ threshold.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -406,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -447,6 +485,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -805,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S21"/>
+  <dimension ref="B2:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -820,56 +864,59 @@
     <col min="6" max="6" width="6.44140625" customWidth="1"/>
     <col min="7" max="7" width="7.5546875" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="13"/>
+    <row r="2" spans="2:20" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
       <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
-    </row>
-    <row r="3" spans="2:19" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="S2" s="13"/>
+    </row>
+    <row r="3" spans="2:20" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="19" t="s">
+      <c r="D3" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="18" t="s">
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="Q3" s="6"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
       <c r="R3" s="6"/>
-      <c r="S3" s="7"/>
-    </row>
-    <row r="4" spans="2:19" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S3" s="6"/>
+      <c r="T3" s="7"/>
+    </row>
+    <row r="4" spans="2:20" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -877,7 +924,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>13</v>
@@ -891,23 +938,26 @@
       <c r="H4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="7"/>
+      <c r="R4" s="8"/>
       <c r="S4" s="7"/>
-    </row>
-    <row r="5" spans="2:19" ht="18" x14ac:dyDescent="0.3">
+      <c r="T4" s="7"/>
+    </row>
+    <row r="5" spans="2:20" ht="18" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -929,21 +979,26 @@
       <c r="H5" s="15">
         <v>21.566510000000001</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="2">
+      <c r="I5" s="16">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="J5" s="5">
+        <v>7.1900000000000006E-2</v>
+      </c>
+      <c r="K5" s="2">
         <v>80</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>79</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>81</v>
       </c>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="7"/>
+      <c r="R5" s="8"/>
       <c r="S5" s="7"/>
-    </row>
-    <row r="6" spans="2:19" ht="18" x14ac:dyDescent="0.3">
+      <c r="T5" s="7"/>
+    </row>
+    <row r="6" spans="2:20" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -965,9 +1020,11 @@
       <c r="H6" s="15">
         <v>23.861560000000001</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="2">
-        <v>100</v>
+      <c r="I6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>21</v>
       </c>
       <c r="K6" s="2">
         <v>100</v>
@@ -975,9 +1032,12 @@
       <c r="L6" s="2">
         <v>100</v>
       </c>
-      <c r="Q6" s="2"/>
-    </row>
-    <row r="7" spans="2:19" ht="18" x14ac:dyDescent="0.3">
+      <c r="M6" s="2">
+        <v>100</v>
+      </c>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="2:20" ht="18" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -999,19 +1059,24 @@
       <c r="H7" s="15">
         <v>59.467800000000004</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="2">
+      <c r="I7" s="16">
+        <v>9.1499999999999998E-2</v>
+      </c>
+      <c r="J7" s="5">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="K7" s="2">
         <v>53</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>57</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>76</v>
       </c>
-      <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="2:19" ht="18" x14ac:dyDescent="0.3">
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="2:20" ht="18" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1033,19 +1098,24 @@
       <c r="H8" s="15">
         <v>66.31362</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2">
+      <c r="I8" s="16">
+        <v>6.5100000000000005E-2</v>
+      </c>
+      <c r="J8" s="16">
+        <v>0.11940000000000001</v>
+      </c>
+      <c r="K8" s="2">
         <v>63</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>36</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>40</v>
       </c>
-      <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="2:19" ht="18" x14ac:dyDescent="0.3">
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="2:20" ht="18" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1067,41 +1137,47 @@
       <c r="H9" s="15">
         <v>51.103940000000001</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="2">
+      <c r="I9" s="16">
+        <v>0.15190000000000001</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1.06E-2</v>
+      </c>
+      <c r="K9" s="2">
         <v>76</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>72</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>81</v>
       </c>
-      <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="2:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="9"/>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="2:20" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
-    </row>
-    <row r="13" spans="2:19" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:19" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="S10" s="9"/>
+    </row>
+    <row r="13" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:20" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
@@ -1109,8 +1185,9 @@
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
-    </row>
-    <row r="15" spans="2:19" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="O14" s="12"/>
+    </row>
+    <row r="15" spans="2:20" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -1118,8 +1195,9 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
-    </row>
-    <row r="16" spans="2:19" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="O15" s="8"/>
+    </row>
+    <row r="16" spans="2:20" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -1127,8 +1205,9 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
-    </row>
-    <row r="17" spans="8:14" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="O16" s="8"/>
+    </row>
+    <row r="17" spans="8:15" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -1136,8 +1215,9 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
-    </row>
-    <row r="18" spans="8:14" ht="18" x14ac:dyDescent="0.3">
+      <c r="O17" s="8"/>
+    </row>
+    <row r="18" spans="8:15" ht="18" x14ac:dyDescent="0.3">
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1145,8 +1225,9 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="8:14" ht="18" x14ac:dyDescent="0.3">
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="8:15" ht="18" x14ac:dyDescent="0.3">
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1154,8 +1235,9 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="8:14" ht="18" x14ac:dyDescent="0.3">
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="8:15" ht="18" x14ac:dyDescent="0.3">
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1163,23 +1245,25 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="8:14" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="8:15" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="H21:N21"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="H21:O21"/>
+    <mergeCell ref="B10:M10"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B2:M2"/>
     <mergeCell ref="D3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>